<commit_message>
Update astimate for TanLoc
</commit_message>
<xml_diff>
--- a/Task/F005_TL/estimate-M2M-F005_TL.xlsx
+++ b/Task/F005_TL/estimate-M2M-F005_TL.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>List of VIP Customer</t>
   </si>
@@ -50,22 +50,19 @@
     <t>Man Day</t>
   </si>
   <si>
-    <t>Create ProductEntity</t>
-  </si>
-  <si>
-    <t>Create ProductRepository</t>
-  </si>
-  <si>
-    <t>Create ProductService /ProductServiceimpl</t>
-  </si>
-  <si>
-    <t>Create Thymeleaf for Ux/Ui</t>
+    <t>Create New Product</t>
+  </si>
+  <si>
+    <t>Design UI</t>
   </si>
   <si>
     <t>Write a function to loading all products</t>
   </si>
   <si>
     <t>Detailed coding  of product functions</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
   </si>
   <si>
     <t>Sum</t>
@@ -1037,11 +1034,11 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="17.1759259259259" customWidth="1"/>
-    <col min="2" max="2" width="9.62962962962963" customWidth="1"/>
-    <col min="3" max="3" width="15.7222222222222" customWidth="1"/>
+    <col min="1" max="1" width="17.175" customWidth="1"/>
+    <col min="2" max="2" width="9.63333333333333" customWidth="1"/>
+    <col min="3" max="3" width="15.725" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1091,15 +1088,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E5:E6"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="46.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="46.775" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1124,11 +1121,11 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="D2">
         <f>C2/8</f>
-        <v>0.1875</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1154,11 +1151,11 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D4">
         <f>C4/8</f>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1169,11 +1166,11 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D5">
         <f>C5/8</f>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1184,39 +1181,24 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f>C6/8</f>
-        <v>0.1875</v>
+        <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
-      </c>
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
-        <v>1.5</v>
-      </c>
-      <c r="D7">
-        <f>C7/8</f>
-        <v>0.1875</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1">
-        <f>SUM(C2:C7)</f>
-        <v>7.5</v>
-      </c>
-      <c r="D8" s="1">
-        <f>SUM(D2:D7)</f>
-        <v>0.9375</v>
+      <c r="C7" s="1">
+        <f>SUM(C2:C6)</f>
+        <v>8.5</v>
+      </c>
+      <c r="D7" s="1">
+        <f>SUM(D2:D6)</f>
+        <v>1.0625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>